<commit_message>
Added student number to student upload file;
</commit_message>
<xml_diff>
--- a/data/files/mschool_student_upload_template.xlsx
+++ b/data/files/mschool_student_upload_template.xlsx
@@ -19,42 +19,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>First Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Last Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>DOB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Gender</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Grade Level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Ethnicity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -88,10 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,42 +437,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>